<commit_message>
feat: update the CCDA to FHIR conversion specification document to update the detailes  of consent, encounter status and observation id in Epic, Medent and AthenaHealth CCDA files #2470
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec - AthenaHealth.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec - AthenaHealth.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" tabRatio="709" firstSheet="3"/>
+    <workbookView windowWidth="28800" windowHeight="12180" tabRatio="709" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="AthenaHealth" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="445">
   <si>
     <t>AthenaHealth CCDA</t>
   </si>
@@ -1728,13 +1728,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">For </t>
     </r>
     <r>
@@ -1756,28 +1749,53 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> CCDs, if the consent document (authorization.consent with code.code = '</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>59284-0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>') is present, then a consent resource with provision.type = "permit" will be generated and if no consent document is present, then a consent resource with provision.type = "deny" will be generated.</t>
+      <t xml:space="preserve"> CCDS, if there is an entry in the Social history section['</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>29762-2'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>] with a consent question (`entry.observation.entryRelationship.observation with code = "105511-0"`) and answer (`entry.observation.entryRelationship.observation.value.code`), then if the `entry.observation.entryRelationship.observation.value.code = '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LA33-6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>' then, a consent resource with provision.type = "permit" will be generated. Otherwise, a consent resource with provision.type = "deny" will be generated.
+If no Observation with code **`105511-0`** is present, then `ClinicalDocument.authorization.consent[code.code='59284-0']` is evaluated:  
+  - If `displayName = "yes"`, the Consent is set to "permit".  
+  - Otherwise, the Consent is set to "deny".
+If neither of the above values is available, the Consent defaults to "deny".</t>
     </r>
   </si>
   <si>
@@ -1804,7 +1822,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Document.authorization.consent.statusCode.code
+      <t xml:space="preserve">Document.component.structuredBody.component.section[code.code='29762-2'].entry.observation.entryRelationship.observation[code.code = '105511-0'].statusCode.code
 </t>
     </r>
     <r>
@@ -2022,7 +2040,7 @@
     <t>dateTime</t>
   </si>
   <si>
-    <t>Document.authorization.consent.effectiveTime.value</t>
+    <t>Document.component.structuredBody.component.section[code.code='29762-2'].entry.observation.entryRelationship.observation[code.code = '105511-0'].effectiveTime.value</t>
   </si>
   <si>
     <t>"dateTime" : "2024-02-23T00:00:00Z",</t>
@@ -2034,7 +2052,7 @@
     <t>provision -&gt; type</t>
   </si>
   <si>
-    <t>Document.authorization.consent.code.displayName</t>
+    <t>Document.component.structuredBody.component.section[code.code='29762-2'].entry.observation.entryRelationship.observation[code.code = '105511-0'].value.code</t>
   </si>
   <si>
     <r>
@@ -2072,7 +2090,222 @@
     </r>
   </si>
   <si>
-    <t>consent -&gt; code -&gt; displayName will be 'deny' or 'permit'.</t>
+    <r>
+      <t>If there is an entry in the Social history section['</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>29762-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'] with a consent question (`entry.observation.entryRelationship.observation with code = '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>105511-0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'`) and answer (`entry.observation.entryRelationship.observation.value.code`), then if the `entry.observation.entryRelationship.observation.value.code` = '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LA33-6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'  then, provision.type = '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>permit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'. Otherwise, provision.type = '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deny</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'.
+If no Observation with code '105511-0' is present, and `ClinicalDocument.authorization.consent[code.code='</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>59284-0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']`.displayName = '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>yes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'`, then provision.type = '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>permit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'.  
+  - Otherwise, provision.type =  '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deny</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'.
+If neither of the above values is available, provision.type will be '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deny</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'.</t>
+    </r>
   </si>
   <si>
     <t>patient -&gt; reference</t>
@@ -2249,36 +2482,32 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">For </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>AthenaHealth</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> CCDA files:
-Document.component.structuredBody.component.section.entry.encounter.statusCode.code</t>
+      <t>First preference will got to ClinicalDocument/ccda:component/ccda:structuredBody/ccda:component/ccda:section[@ID='encounters']/ccda:entry[1]/ccda:encounter[1]/ccda:statusCode/@code
+If the above path is not present, the `moodCode` is evaluated from:  
+ClinicalDocument/ccda:component/ccda:structuredBody/ccda:component/ccda:section[@ID='encounters']/ccda:entry[1]/ccda:encounter[1]/@moodCode
+  - If `moodCode = '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EVN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'`, the Encounter Status is set to "finished".  
+If neither of the above values is available, the Encounter Status is set to "unknown".</t>
     </r>
   </si>
   <si>
@@ -3909,7 +4138,97 @@
     </r>
   </si>
   <si>
-    <t>"id" : "N6645918CUMC20250121T1024400530",</t>
+    <r>
+      <t>Combine the Facility ID obtained from the header variable '</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>X-TechBD-Facility-ID'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t> with the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> id.extension</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> value from the Observation element.</t>
+    </r>
+  </si>
+  <si>
+    <t>"id": "ACPNY-c6a74afc-5782-47e0-84b8-08e143d27c91"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>id.extension</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is not available then</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 'id.root'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> will be taken.</t>
+    </r>
   </si>
   <si>
     <t>"http://shinny.org/us/ny/hrsn/StructureDefinition/shinny-observation-screening-response"</t>
@@ -4587,6 +4906,9 @@
       </rPr>
       <t xml:space="preserve"> CCDA files, the Observations are taken from Document.component.structuredBody.component.section[code[@code = '29762-2']].entry.observation.entryRelationship.observation</t>
     </r>
+  </si>
+  <si>
+    <t>"id" : "N6645918CUMC20250121T1024400530",</t>
   </si>
   <si>
     <t>Provided the fixed value, "en"</t>
@@ -5212,7 +5534,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5433,6 +5755,30 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -5447,27 +5793,23 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Consolas"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF00B050"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <sz val="10.5"/>
+      <color rgb="FF00B050"/>
+      <name val="Segoe UI"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF00B050"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="35">
@@ -5932,7 +6274,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -5958,9 +6300,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -6555,24 +6894,24 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="8.88571428571429" style="25"/>
+    <col min="1" max="1" width="8.88571428571429" style="24"/>
     <col min="2" max="2" width="35.2190476190476" customWidth="1"/>
     <col min="3" max="3" width="92.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="25">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -6583,10 +6922,10 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="25">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
@@ -6594,10 +6933,10 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="25">
+      <c r="A5" s="24">
         <v>3</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
@@ -6605,10 +6944,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="25">
+      <c r="A6" s="24">
         <v>4</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
@@ -6616,10 +6955,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="25">
+      <c r="A7" s="24">
         <v>5</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="26" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
@@ -6673,10 +7012,10 @@
     </row>
     <row r="2" ht="29" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -6687,7 +7026,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" ht="60" spans="2:7">
@@ -6698,7 +7037,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
@@ -6716,27 +7055,27 @@
       <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>425</v>
+      <c r="C6" s="4" t="s">
+        <v>428</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>426</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>427</v>
+        <v>429</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>428</v>
+      <c r="C7" s="10" t="s">
+        <v>431</v>
       </c>
       <c r="D7" t="s">
-        <v>429</v>
-      </c>
-      <c r="E7" s="12"/>
+        <v>432</v>
+      </c>
+      <c r="E7" s="11"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" customFormat="1" ht="120" spans="2:5">
@@ -6744,13 +7083,13 @@
         <v>80</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="D8" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>431</v>
+      <c r="E8" s="13" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="9" customFormat="1" ht="60" spans="2:5">
@@ -6758,9 +7097,9 @@
         <v>84</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>432</v>
-      </c>
-      <c r="D9" s="13"/>
+        <v>435</v>
+      </c>
+      <c r="D9" s="12"/>
       <c r="E9" s="4"/>
     </row>
     <row r="10" customFormat="1" spans="2:5">
@@ -6768,9 +7107,9 @@
         <v>86</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="D10" s="13"/>
+        <v>436</v>
+      </c>
+      <c r="D10" s="12"/>
       <c r="E10" s="4"/>
     </row>
     <row r="11" customFormat="1" spans="2:5">
@@ -6778,9 +7117,9 @@
         <v>88</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>434</v>
-      </c>
-      <c r="D11" s="13"/>
+        <v>437</v>
+      </c>
+      <c r="D11" s="12"/>
       <c r="E11" s="4"/>
     </row>
     <row r="12" customFormat="1" spans="2:5">
@@ -6788,9 +7127,9 @@
         <v>90</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>435</v>
-      </c>
-      <c r="D12" s="13"/>
+        <v>438</v>
+      </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="4"/>
     </row>
     <row r="13" customFormat="1" spans="2:5">
@@ -6798,9 +7137,9 @@
         <v>92</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>436</v>
-      </c>
-      <c r="D13" s="13"/>
+        <v>439</v>
+      </c>
+      <c r="D13" s="12"/>
       <c r="E13" s="4"/>
     </row>
     <row r="14" customFormat="1" spans="2:5">
@@ -6808,19 +7147,19 @@
         <v>94</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>437</v>
-      </c>
-      <c r="D14" s="13"/>
+        <v>440</v>
+      </c>
+      <c r="D14" s="12"/>
       <c r="E14" s="4"/>
     </row>
     <row r="15" customFormat="1" spans="2:5">
       <c r="B15" s="4" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="D15" s="13"/>
+        <v>442</v>
+      </c>
+      <c r="D15" s="12"/>
       <c r="E15" s="4"/>
     </row>
     <row r="16" customFormat="1" spans="2:6">
@@ -6830,8 +7169,8 @@
       <c r="C16" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>440</v>
+      <c r="D16" s="14" t="s">
+        <v>443</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="4"/>
@@ -6841,9 +7180,9 @@
         <v>191</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>441</v>
-      </c>
-      <c r="D17" s="15"/>
+        <v>444</v>
+      </c>
+      <c r="D17" s="14"/>
       <c r="E17" s="8"/>
       <c r="F17" s="4"/>
     </row>
@@ -6985,7 +7324,7 @@
       <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>34</v>
       </c>
     </row>
@@ -7004,7 +7343,7 @@
       <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="17" t="s">
+      <c r="E18" s="16" t="s">
         <v>39</v>
       </c>
     </row>
@@ -7012,19 +7351,19 @@
       <c r="B19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E19" s="11"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" ht="45" spans="2:5">
       <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E20" s="11"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" ht="30" spans="2:5">
       <c r="B21" s="4" t="s">
@@ -7064,19 +7403,19 @@
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>46</v>
       </c>
     </row>
@@ -7095,7 +7434,7 @@
       </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -7107,7 +7446,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1"/>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -7115,7 +7454,7 @@
       </c>
     </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -7140,7 +7479,7 @@
       <c r="C8" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>56</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -7148,13 +7487,13 @@
       </c>
     </row>
     <row r="9" spans="2:4">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" spans="2:4">
       <c r="B10" s="4" t="s">
@@ -7163,29 +7502,29 @@
       <c r="C10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="2:4">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>63</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>66</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>67</v>
       </c>
     </row>
@@ -7196,7 +7535,7 @@
       <c r="C13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>70</v>
       </c>
     </row>
@@ -7218,18 +7557,18 @@
       <c r="C15" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="16" spans="2:4">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>79</v>
       </c>
     </row>
@@ -7240,10 +7579,10 @@
       <c r="C17" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>83</v>
       </c>
     </row>
@@ -7254,7 +7593,7 @@
       <c r="C18" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="13"/>
+      <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:4">
       <c r="B19" s="4" t="s">
@@ -7263,7 +7602,7 @@
       <c r="C19" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="13"/>
+      <c r="D19" s="12"/>
     </row>
     <row r="20" spans="2:4">
       <c r="B20" s="4" t="s">
@@ -7272,7 +7611,7 @@
       <c r="C20" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="13"/>
+      <c r="D20" s="12"/>
     </row>
     <row r="21" spans="2:4">
       <c r="B21" s="4" t="s">
@@ -7281,7 +7620,7 @@
       <c r="C21" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="13"/>
+      <c r="D21" s="12"/>
     </row>
     <row r="22" spans="2:4">
       <c r="B22" s="4" t="s">
@@ -7290,7 +7629,7 @@
       <c r="C22" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="13"/>
+      <c r="D22" s="12"/>
     </row>
     <row r="23" spans="2:4">
       <c r="B23" s="4" t="s">
@@ -7299,7 +7638,7 @@
       <c r="C23" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="13"/>
+      <c r="D23" s="12"/>
     </row>
     <row r="24" ht="48" customHeight="1" spans="2:5">
       <c r="B24" s="4" t="s">
@@ -7327,7 +7666,7 @@
       <c r="C26" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -7338,7 +7677,7 @@
       <c r="C27" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="12" t="s">
         <v>106</v>
       </c>
       <c r="E27" s="8" t="s">
@@ -7352,7 +7691,7 @@
       <c r="C28" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="15"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="2:5">
@@ -7362,7 +7701,7 @@
       <c r="C29" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D29" s="15"/>
+      <c r="D29" s="14"/>
       <c r="E29" s="8"/>
     </row>
     <row r="30" ht="30" spans="2:5">
@@ -7372,7 +7711,7 @@
       <c r="C30" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="15"/>
+      <c r="D30" s="14"/>
       <c r="E30" s="8"/>
     </row>
     <row r="31" spans="2:5">
@@ -7382,7 +7721,7 @@
       <c r="C31" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="15"/>
+      <c r="D31" s="14"/>
       <c r="E31" s="8"/>
     </row>
     <row r="32" ht="45" spans="2:5">
@@ -7392,7 +7731,7 @@
       <c r="C32" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>116</v>
       </c>
       <c r="E32" s="8" t="s">
@@ -7406,7 +7745,7 @@
       <c r="C33" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D33" s="15"/>
+      <c r="D33" s="14"/>
     </row>
     <row r="34" spans="2:4">
       <c r="B34" s="4" t="s">
@@ -7415,7 +7754,7 @@
       <c r="C34" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D34" s="15"/>
+      <c r="D34" s="14"/>
     </row>
     <row r="35" ht="30" spans="2:4">
       <c r="B35" s="4" t="s">
@@ -7424,7 +7763,7 @@
       <c r="C35" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D35" s="15"/>
+      <c r="D35" s="14"/>
     </row>
     <row r="36" spans="2:4">
       <c r="B36" s="4" t="s">
@@ -7433,7 +7772,7 @@
       <c r="C36" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="15"/>
+      <c r="D36" s="14"/>
     </row>
     <row r="37" spans="2:4">
       <c r="B37" s="4" t="s">
@@ -7442,7 +7781,7 @@
       <c r="C37" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="14" t="s">
         <v>123</v>
       </c>
     </row>
@@ -7453,8 +7792,8 @@
       <c r="C38" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="28" t="s">
+      <c r="D38" s="14"/>
+      <c r="E38" s="27" t="s">
         <v>125</v>
       </c>
     </row>
@@ -7462,7 +7801,7 @@
       <c r="B39" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="10" t="s">
         <v>127</v>
       </c>
       <c r="F39" s="4" t="s">
@@ -7473,7 +7812,7 @@
       <c r="B40" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>130</v>
       </c>
       <c r="F40" s="4" t="s">
@@ -7481,31 +7820,31 @@
       </c>
     </row>
     <row r="41" spans="2:4">
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="15" t="s">
         <v>132</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="11"/>
+      <c r="D41" s="10"/>
     </row>
     <row r="42" spans="2:4">
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="15" t="s">
         <v>134</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D42" s="11"/>
+      <c r="D42" s="10"/>
     </row>
     <row r="43" spans="2:4">
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="15" t="s">
         <v>136</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D43" s="11"/>
+      <c r="D43" s="10"/>
     </row>
     <row r="44" spans="2:4">
       <c r="B44" s="4" t="s">
@@ -7514,30 +7853,30 @@
       <c r="C44" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="D44" s="11"/>
+      <c r="D44" s="10"/>
     </row>
     <row r="45" ht="195" spans="2:5">
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="D45" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E45" s="17" t="s">
+      <c r="E45" s="16" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="46" ht="195" spans="2:5">
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C46" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="D46" s="10" t="s">
         <v>145</v>
       </c>
       <c r="E46" s="8" t="s">
@@ -7545,16 +7884,16 @@
       </c>
     </row>
     <row r="47" ht="195" spans="2:5">
-      <c r="B47" s="16" t="s">
+      <c r="B47" s="15" t="s">
         <v>147</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D47" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="E47" s="23"/>
+      <c r="E47" s="22"/>
     </row>
     <row r="48" customFormat="1" spans="2:5">
       <c r="B48" s="4" t="s">
@@ -7563,7 +7902,7 @@
       <c r="C48" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D48" s="11"/>
+      <c r="D48" s="10"/>
       <c r="E48" s="4"/>
     </row>
     <row r="49" customFormat="1" spans="2:5">
@@ -7573,7 +7912,7 @@
       <c r="C49" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D49" s="11"/>
+      <c r="D49" s="10"/>
       <c r="E49" s="4"/>
     </row>
     <row r="50" customFormat="1" spans="2:5">
@@ -7583,7 +7922,7 @@
       <c r="C50" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D50" s="11"/>
+      <c r="D50" s="10"/>
       <c r="E50" s="4"/>
     </row>
     <row r="51" customFormat="1" spans="2:5">
@@ -7593,17 +7932,17 @@
       <c r="C51" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="D51" s="11"/>
+      <c r="D51" s="10"/>
       <c r="E51" s="4"/>
     </row>
     <row r="52" ht="150" spans="2:5">
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C52" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="10" t="s">
         <v>158</v>
       </c>
       <c r="E52" s="8" t="s">
@@ -7614,10 +7953,10 @@
       <c r="B53" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="D53" s="11"/>
+      <c r="D53" s="10"/>
       <c r="E53" s="8"/>
     </row>
     <row r="54" customFormat="1" spans="2:5">
@@ -7627,7 +7966,7 @@
       <c r="C54" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D54" s="11"/>
+      <c r="D54" s="10"/>
       <c r="E54" s="8"/>
     </row>
     <row r="55" customFormat="1" spans="2:5">
@@ -7637,7 +7976,7 @@
       <c r="C55" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="D55" s="11"/>
+      <c r="D55" s="10"/>
       <c r="E55" s="8"/>
     </row>
     <row r="56" customFormat="1" spans="2:5">
@@ -7647,7 +7986,7 @@
       <c r="C56" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D56" s="11"/>
+      <c r="D56" s="10"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" customFormat="1" spans="2:5">
@@ -7657,30 +7996,30 @@
       <c r="C57" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D57" s="11"/>
+      <c r="D57" s="10"/>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="D58" s="11"/>
+      <c r="D58" s="10"/>
       <c r="E58" s="8"/>
     </row>
     <row r="59" ht="180" spans="2:5">
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D59" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="E59" s="16" t="s">
         <v>172</v>
       </c>
     </row>
@@ -7688,7 +8027,7 @@
       <c r="B60" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="D60" s="11" t="s">
+      <c r="D60" s="10" t="s">
         <v>174</v>
       </c>
       <c r="F60" s="4" t="s">
@@ -7702,7 +8041,7 @@
       <c r="C61" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D61" s="11"/>
+      <c r="D61" s="10"/>
       <c r="F61" s="4"/>
     </row>
     <row r="62" spans="2:6">
@@ -7712,15 +8051,15 @@
       <c r="C62" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D62" s="11"/>
+      <c r="D62" s="10"/>
       <c r="F62" s="4"/>
     </row>
     <row r="63" ht="210" spans="2:6">
       <c r="B63" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D63" s="11"/>
-      <c r="E63" s="14" t="s">
+      <c r="D63" s="10"/>
+      <c r="E63" s="13" t="s">
         <v>181</v>
       </c>
       <c r="F63" s="4"/>
@@ -7729,7 +8068,7 @@
       <c r="B64" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="D64" s="13" t="s">
+      <c r="D64" s="12" t="s">
         <v>183</v>
       </c>
       <c r="F64" s="4" t="s">
@@ -7743,7 +8082,7 @@
       <c r="C65" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D65" s="13"/>
+      <c r="D65" s="12"/>
     </row>
     <row r="66" ht="40" customHeight="1" spans="2:4">
       <c r="B66" s="4" t="s">
@@ -7752,7 +8091,7 @@
       <c r="C66" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D66" s="13"/>
+      <c r="D66" s="12"/>
     </row>
     <row r="67" spans="2:4">
       <c r="B67" s="4" t="s">
@@ -7761,7 +8100,7 @@
       <c r="C67" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D67" s="15" t="s">
+      <c r="D67" s="14" t="s">
         <v>190</v>
       </c>
     </row>
@@ -7772,7 +8111,7 @@
       <c r="C68" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="D68" s="15"/>
+      <c r="D68" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7794,8 +8133,8 @@
   <sheetPr/>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -7828,7 +8167,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" ht="33" customHeight="1" spans="1:5">
+    <row r="2" ht="105" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -7876,19 +8215,19 @@
       <c r="C6" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" ht="120" spans="2:6">
       <c r="B7" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>199</v>
       </c>
       <c r="D7" t="s">
         <v>200</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>201</v>
       </c>
       <c r="F7" s="4"/>
@@ -7900,7 +8239,7 @@
       <c r="C8" t="s">
         <v>203</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>204</v>
       </c>
       <c r="E8" s="8" t="s">
@@ -7914,7 +8253,7 @@
       <c r="C9" t="s">
         <v>207</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="8" t="s">
         <v>205</v>
       </c>
@@ -7926,7 +8265,7 @@
       <c r="C10" t="s">
         <v>209</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="8" t="s">
         <v>205</v>
       </c>
@@ -7938,7 +8277,7 @@
       <c r="C11" t="s">
         <v>211</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>212</v>
       </c>
       <c r="E11" s="8" t="s">
@@ -7967,11 +8306,11 @@
         <v>205</v>
       </c>
     </row>
-    <row r="14" ht="30" spans="2:5">
+    <row r="14" ht="45" spans="2:5">
       <c r="B14" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>218</v>
       </c>
       <c r="D14" t="s">
@@ -7981,17 +8320,17 @@
         <v>220</v>
       </c>
     </row>
-    <row r="15" ht="45" spans="2:5">
+    <row r="15" ht="255" spans="2:5">
       <c r="B15" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="16" t="s">
         <v>224</v>
       </c>
     </row>
@@ -8026,7 +8365,7 @@
       <c r="C18" t="s">
         <v>232</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>233</v>
       </c>
       <c r="E18" s="8" t="s">
@@ -8066,7 +8405,7 @@
       <c r="C21" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>239</v>
       </c>
       <c r="E21" s="8"/>
@@ -8079,7 +8418,7 @@
       <c r="C22" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="D22" s="15"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="8"/>
       <c r="F22" s="4"/>
     </row>
@@ -8100,7 +8439,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -8120,7 +8459,7 @@
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -8169,7 +8508,7 @@
     </row>
     <row r="5" customFormat="1" spans="1:6">
       <c r="A5" s="1"/>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -8180,7 +8519,7 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" customFormat="1" ht="30" spans="2:6">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -8190,17 +8529,17 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" ht="165" spans="2:5">
+    <row r="7" ht="255" spans="2:5">
       <c r="B7" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>246</v>
       </c>
       <c r="D7" t="s">
         <v>247</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>248</v>
       </c>
     </row>
@@ -8211,10 +8550,10 @@
       <c r="C8" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" ht="30" spans="2:5">
       <c r="B9" s="5" t="s">
@@ -8223,8 +8562,8 @@
       <c r="C9" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="23"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="22"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
@@ -8233,17 +8572,17 @@
       <c r="C10" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" ht="30" spans="2:4">
       <c r="B11" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>258</v>
       </c>
     </row>
@@ -8251,8 +8590,8 @@
       <c r="B12" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="13" t="s">
         <v>260</v>
       </c>
     </row>
@@ -8263,7 +8602,7 @@
       <c r="C13" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="D13" s="13"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" customFormat="1" spans="2:3">
       <c r="B14" t="s">
@@ -8280,7 +8619,7 @@
       <c r="C15" t="s">
         <v>226</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>266</v>
       </c>
     </row>
@@ -8299,7 +8638,7 @@
       <c r="C17" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>271</v>
       </c>
     </row>
@@ -8318,7 +8657,7 @@
       <c r="C19" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>276</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -8332,7 +8671,7 @@
       <c r="C20" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="E20" s="18"/>
+      <c r="E20" s="17"/>
     </row>
     <row r="21" ht="409.5" spans="2:5">
       <c r="B21" t="s">
@@ -8341,7 +8680,7 @@
       <c r="C21" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>282</v>
       </c>
     </row>
@@ -8352,7 +8691,7 @@
       <c r="C22" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="E22" s="21"/>
+      <c r="E22" s="20"/>
     </row>
     <row r="23" ht="66" customHeight="1" spans="2:5">
       <c r="B23" t="s">
@@ -8361,7 +8700,7 @@
       <c r="C23" t="s">
         <v>286</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>287</v>
       </c>
       <c r="E23" s="4"/>
@@ -8373,7 +8712,7 @@
       <c r="C24" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="D24" s="11"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="4"/>
     </row>
     <row r="25" customFormat="1" spans="2:4">
@@ -8383,7 +8722,7 @@
       <c r="C25" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="14" t="s">
         <v>290</v>
       </c>
     </row>
@@ -8394,7 +8733,7 @@
       <c r="C26" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="D26" s="15"/>
+      <c r="D26" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -8505,7 +8844,7 @@
       <c r="E7" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>298</v>
       </c>
     </row>
@@ -8513,10 +8852,10 @@
       <c r="B8" t="s">
         <v>299</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>300</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>301</v>
       </c>
     </row>
@@ -8527,7 +8866,7 @@
       <c r="C9" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="D9" s="11"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" ht="30" spans="2:5">
@@ -8537,7 +8876,7 @@
       <c r="C10" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="10"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" ht="30" spans="2:5">
@@ -8547,7 +8886,7 @@
       <c r="C11" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" ht="30" spans="2:5">
@@ -8557,17 +8896,17 @@
       <c r="C12" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="8"/>
     </row>
     <row r="13" customFormat="1" ht="66" customHeight="1" spans="2:4">
       <c r="B13" t="s">
         <v>309</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>311</v>
       </c>
     </row>
@@ -8578,8 +8917,8 @@
       <c r="C14" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="21"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="20"/>
     </row>
     <row r="15" customFormat="1" ht="30" spans="2:5">
       <c r="B15" s="4" t="s">
@@ -8588,8 +8927,8 @@
       <c r="C15" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="21"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="20"/>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:5">
       <c r="B16" s="4" t="s">
@@ -8598,7 +8937,7 @@
       <c r="C16" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="11"/>
+      <c r="D16" s="10"/>
       <c r="E16" s="4"/>
     </row>
     <row r="17" customFormat="1" ht="30" spans="2:4">
@@ -8608,16 +8947,16 @@
       <c r="C17" s="4" t="s">
         <v>318</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="10"/>
     </row>
     <row r="18" ht="60" spans="2:5">
       <c r="B18" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="16" t="s">
         <v>320</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>321</v>
       </c>
       <c r="E18" s="4" t="s">
@@ -8628,7 +8967,7 @@
       <c r="B19" t="s">
         <v>323</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>324</v>
       </c>
       <c r="F19" s="8" t="s">
@@ -8640,7 +8979,7 @@
         <v>326</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="11"/>
+      <c r="D20" s="10"/>
       <c r="F20" s="8" t="s">
         <v>327</v>
       </c>
@@ -8650,7 +8989,7 @@
         <v>96</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>328</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -8665,7 +9004,7 @@
       <c r="C22" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="D22" s="11"/>
+      <c r="D22" s="10"/>
       <c r="F22" s="4"/>
     </row>
     <row r="23" customFormat="1" ht="195" spans="2:6">
@@ -8675,8 +9014,8 @@
       <c r="C23" s="4" t="s">
         <v>330</v>
       </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="14" t="s">
+      <c r="D23" s="10"/>
+      <c r="E23" s="13" t="s">
         <v>103</v>
       </c>
       <c r="F23" s="4"/>
@@ -8688,7 +9027,7 @@
       <c r="C24" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>332</v>
       </c>
       <c r="E24" s="4"/>
@@ -8701,7 +9040,7 @@
       <c r="C25" s="4" t="s">
         <v>333</v>
       </c>
-      <c r="D25" s="11"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
     </row>
@@ -8712,7 +9051,7 @@
       <c r="C26" s="4" t="s">
         <v>334</v>
       </c>
-      <c r="D26" s="11"/>
+      <c r="D26" s="10"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
     </row>
@@ -8723,7 +9062,7 @@
       <c r="C27" s="4" t="s">
         <v>335</v>
       </c>
-      <c r="D27" s="11"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
     </row>
@@ -8734,7 +9073,7 @@
       <c r="C28" s="4" t="s">
         <v>336</v>
       </c>
-      <c r="D28" s="11"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
     </row>
@@ -8745,7 +9084,7 @@
       <c r="C29" s="4" t="s">
         <v>337</v>
       </c>
-      <c r="D29" s="11"/>
+      <c r="D29" s="10"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
     </row>
@@ -8756,7 +9095,7 @@
       <c r="C30" s="4" t="s">
         <v>338</v>
       </c>
-      <c r="D30" s="11"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
     </row>
@@ -8767,7 +9106,7 @@
       <c r="C31" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="14" t="s">
         <v>339</v>
       </c>
     </row>
@@ -8778,7 +9117,7 @@
       <c r="C32" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="D32" s="15"/>
+      <c r="D32" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -8834,7 +9173,7 @@
       </c>
     </row>
     <row r="2" ht="45" spans="1:1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="19" t="s">
         <v>341</v>
       </c>
     </row>
@@ -8861,7 +9200,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1"/>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -8872,7 +9211,7 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" ht="30" spans="2:6">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -8903,7 +9242,7 @@
       <c r="D8" t="s">
         <v>347</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>348</v>
       </c>
     </row>
@@ -8914,7 +9253,7 @@
       <c r="C9" s="4" t="s">
         <v>350</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>351</v>
       </c>
     </row>
@@ -8925,7 +9264,7 @@
       <c r="C10" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5" t="s">
@@ -8934,7 +9273,7 @@
       <c r="C11" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="10"/>
       <c r="E11" s="8"/>
     </row>
     <row r="12" ht="30" spans="2:4">
@@ -8944,7 +9283,7 @@
       <c r="C12" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" ht="38" customHeight="1" spans="2:4">
       <c r="B13" s="4" t="s">
@@ -8953,7 +9292,7 @@
       <c r="C13" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>358</v>
       </c>
     </row>
@@ -8964,7 +9303,7 @@
       <c r="C14" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" ht="153" customHeight="1" spans="2:5">
       <c r="B15" s="4" t="s">
@@ -8973,7 +9312,7 @@
       <c r="C15" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="8" t="s">
         <v>363</v>
       </c>
@@ -8985,7 +9324,7 @@
       <c r="C16" t="s">
         <v>226</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>266</v>
       </c>
     </row>
@@ -9018,7 +9357,7 @@
       <c r="D19" t="s">
         <v>369</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="17" t="s">
         <v>370</v>
       </c>
     </row>
@@ -9029,7 +9368,7 @@
       <c r="C20" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>371</v>
       </c>
     </row>
@@ -9040,7 +9379,7 @@
       <c r="C21" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="D21" s="15"/>
+      <c r="D21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9059,7 +9398,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -9102,7 +9441,7 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="19"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1"/>
@@ -9113,21 +9452,24 @@
         <v>342</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" ht="46.5" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
+      <c r="C4" s="16" t="s">
+        <v>374</v>
       </c>
       <c r="D4" t="s">
-        <v>374</v>
+        <v>375</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>376</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
       <c r="A5" s="1"/>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -9138,11 +9480,11 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" customFormat="1" ht="30" spans="2:6">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -9164,24 +9506,24 @@
         <v>198</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D8" t="s">
         <v>347</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="9" ht="139" customHeight="1" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>379</v>
+        <v>380</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="10" ht="45" spans="2:5">
@@ -9189,11 +9531,11 @@
         <v>215</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="8" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" ht="210" spans="2:5">
@@ -9201,8 +9543,8 @@
         <v>210</v>
       </c>
       <c r="D11" s="6"/>
-      <c r="E11" s="12" t="s">
-        <v>382</v>
+      <c r="E11" s="11" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="12" ht="210" spans="2:5">
@@ -9210,31 +9552,31 @@
         <v>213</v>
       </c>
       <c r="D12" s="6"/>
-      <c r="E12" s="12" t="s">
-        <v>383</v>
+      <c r="E12" s="11" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="2:5">
       <c r="B13" s="5" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="8" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
     </row>
     <row r="14" ht="84" customHeight="1" spans="2:5">
       <c r="B14" s="5" t="s">
         <v>349</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="D14" s="11" t="s">
+      <c r="C14" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>351</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>387</v>
+      <c r="E14" s="16" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="15" spans="2:5">
@@ -9244,8 +9586,8 @@
       <c r="C15" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="9"/>
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="5" t="s">
@@ -9254,19 +9596,19 @@
       <c r="C16" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="9"/>
     </row>
     <row r="17" ht="30" spans="2:5">
       <c r="B17" s="5" t="s">
         <v>355</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="D17" s="11"/>
+        <v>390</v>
+      </c>
+      <c r="D17" s="10"/>
       <c r="E17" s="8" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="18" ht="105" spans="2:5">
@@ -9274,13 +9616,13 @@
         <v>356</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>391</v>
-      </c>
-      <c r="E18" s="17" t="s">
         <v>392</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="19" ht="30" spans="2:3">
@@ -9288,7 +9630,7 @@
         <v>359</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
     </row>
     <row r="20" ht="30" spans="2:3">
@@ -9301,35 +9643,35 @@
     </row>
     <row r="21" ht="37" customHeight="1" spans="2:5">
       <c r="B21" s="5" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>396</v>
+        <v>397</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>398</v>
       </c>
       <c r="E21" s="8"/>
     </row>
     <row r="22" ht="75" spans="2:5">
       <c r="B22" s="5" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C22" t="s">
-        <v>398</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="12" t="s">
-        <v>399</v>
+        <v>400</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="11" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="23" ht="45" spans="2:5">
       <c r="B23" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="12" t="s">
-        <v>401</v>
+        <v>402</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="11" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="24" ht="75" spans="2:4">
@@ -9339,7 +9681,7 @@
       <c r="C24" t="s">
         <v>226</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>266</v>
       </c>
     </row>
@@ -9353,13 +9695,13 @@
     </row>
     <row r="26" ht="45" spans="2:4">
       <c r="B26" s="5" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C26" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="27" ht="210" spans="2:5">
@@ -9370,19 +9712,19 @@
       <c r="D27" t="s">
         <v>366</v>
       </c>
-      <c r="E27" s="17" t="s">
-        <v>405</v>
+      <c r="E27" s="16" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="28" ht="45" spans="2:4">
       <c r="B28" s="5" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>229</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="29" spans="2:6">
@@ -9404,8 +9746,8 @@
       <c r="C30" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D30" s="15" t="s">
-        <v>408</v>
+      <c r="D30" s="14" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="31" ht="46" customHeight="1" spans="2:4">
@@ -9415,7 +9757,7 @@
       <c r="C31" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="D31" s="15"/>
+      <c r="D31" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -9474,7 +9816,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9499,12 +9841,12 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>374</v>
+        <v>412</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:6">
       <c r="A5" s="1"/>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -9515,11 +9857,11 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" customFormat="1" ht="30" spans="2:6">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -9533,7 +9875,7 @@
         <v>53</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>345</v>
@@ -9544,24 +9886,24 @@
         <v>198</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="D8" t="s">
         <v>347</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="9" ht="409" customHeight="1" spans="2:5">
       <c r="B9" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>411</v>
+        <v>379</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>414</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" ht="165" spans="2:5">
@@ -9571,11 +9913,11 @@
       <c r="C10" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>413</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>414</v>
+      <c r="D10" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>417</v>
       </c>
     </row>
     <row r="11" ht="180" spans="2:5">
@@ -9583,8 +9925,8 @@
         <v>352</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="E11" s="12" t="s">
-        <v>415</v>
+      <c r="E11" s="11" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="12" ht="150" spans="2:5">
@@ -9592,8 +9934,8 @@
         <v>354</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="E12" s="12" t="s">
-        <v>416</v>
+      <c r="E12" s="11" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="13" ht="75" spans="2:4">
@@ -9603,7 +9945,7 @@
       <c r="C13" t="s">
         <v>226</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>266</v>
       </c>
     </row>
@@ -9617,13 +9959,13 @@
     </row>
     <row r="15" ht="45" spans="2:4">
       <c r="B15" s="5" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C15" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
     </row>
     <row r="16" ht="210" spans="2:5">
@@ -9634,19 +9976,19 @@
       <c r="D16" t="s">
         <v>366</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>405</v>
+      <c r="E16" s="16" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="17" ht="45" spans="2:4">
       <c r="B17" s="5" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>229</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" spans="2:6">
@@ -9657,21 +9999,21 @@
         <v>369</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>417</v>
-      </c>
-      <c r="F18" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="F18" s="17" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="19" ht="165" spans="2:5">
       <c r="B19" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="E19" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -9681,8 +10023,8 @@
       <c r="C20" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D20" s="15" t="s">
-        <v>408</v>
+      <c r="D20" s="14" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="21" ht="46" customHeight="1" spans="2:4">
@@ -9692,7 +10034,7 @@
       <c r="C21" s="4" t="s">
         <v>372</v>
       </c>
-      <c r="D21" s="15"/>
+      <c r="D21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
docs: updated CCDA to FHIR converion specification documents with changes in observation resourced ID and Organization identifier #2470
</commit_message>
<xml_diff>
--- a/support/specifications/ccda/CCDA to FHIR Conversion Spec - AthenaHealth.xlsx
+++ b/support/specifications/ccda/CCDA to FHIR Conversion Spec - AthenaHealth.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" tabRatio="709" firstSheet="3" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="12180" tabRatio="709" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="AthenaHealth" sheetId="11" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="445">
   <si>
     <t>AthenaHealth CCDA</t>
   </si>
@@ -1728,6 +1728,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">For </t>
     </r>
     <r>
@@ -2091,6 +2098,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>If there is an entry in the Social history section['</t>
     </r>
     <r>
@@ -2482,6 +2496,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>First preference will got to ClinicalDocument/ccda:component/ccda:structuredBody/ccda:component/ccda:section[@ID='encounters']/ccda:entry[1]/ccda:encounter[1]/ccda:statusCode/@code
 If the above path is not present, the `moodCode` is evaluated from:  
 ClinicalDocument/ccda:component/ccda:structuredBody/ccda:component/ccda:section[@ID='encounters']/ccda:entry[1]/ccda:encounter[1]/@moodCode
@@ -3403,6 +3424,9 @@
     </r>
   </si>
   <si>
+    <t>Both TAX and NPI numbers will be added to the Identifier if available.</t>
+  </si>
+  <si>
     <t>identifier (TAX) -&gt; system</t>
   </si>
   <si>
@@ -4149,25 +4173,64 @@
         <rFont val="Consolas"/>
         <charset val="134"/>
       </rPr>
-      <t>X-TechBD-Facility-ID'</t>
-    </r>
-    <r>
-      <rPr>
+      <t xml:space="preserve">X-TechBD-Facility-ID' </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t>and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="10.5"/>
         <color rgb="FF00B050"/>
         <rFont val="Segoe UI"/>
         <charset val="134"/>
       </rPr>
-      <t> with the</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+      <t>code.code</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Consolas"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
         <sz val="10.5"/>
         <color rgb="FF00B050"/>
         <rFont val="Segoe UI"/>
         <charset val="134"/>
       </rPr>
+      <t>with the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve"> id.extension</t>
     </r>
     <r>
@@ -4177,58 +4240,52 @@
         <rFont val="Segoe UI"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> value from the Observation element.</t>
-    </r>
-  </si>
-  <si>
-    <t>"id": "ACPNY-c6a74afc-5782-47e0-84b8-08e143d27c91"</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">If </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
+      <t xml:space="preserve"> value from the Observation element.
+If </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
       </rPr>
       <t>id.extension</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> is not available then</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 'id.root'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> will be taken.</t>
-    </r>
+        <sz val="10.5"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> is not available then add </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10.5"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t>effectiveDateTime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Segoe UI"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> calculated.</t>
+    </r>
+  </si>
+  <si>
+    <t>"id": "ACPNY-96778-6-20260217000000"
+OR
+"id": "ACPNY-96778-6-flo1570000081-5810220439-97066-Z549669"</t>
   </si>
   <si>
     <t>"http://shinny.org/us/ny/hrsn/StructureDefinition/shinny-observation-screening-response"</t>
@@ -5534,7 +5591,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5755,7 +5812,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -5763,7 +5820,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -5771,7 +5827,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF00B050"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -5787,6 +5843,7 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -5799,13 +5856,19 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FF00B050"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10.5"/>
       <color rgb="FF00B050"/>
       <name val="Segoe UI"/>
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="10.5"/>
       <color rgb="FF00B050"/>
       <name val="Segoe UI"/>
@@ -6274,7 +6337,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -6331,6 +6394,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -6900,18 +6966,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="8.88571428571429" style="24"/>
+    <col min="1" max="1" width="8.88571428571429" style="25"/>
     <col min="2" max="2" width="35.2190476190476" customWidth="1"/>
     <col min="3" max="3" width="92.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="24">
+      <c r="A3" s="25">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -6922,7 +6988,7 @@
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="24">
+      <c r="A4" s="25">
         <v>2</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -6933,7 +6999,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="24">
+      <c r="A5" s="25">
         <v>3</v>
       </c>
       <c r="B5" s="17" t="s">
@@ -6944,10 +7010,10 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="24">
+      <c r="A6" s="25">
         <v>4</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
@@ -6955,10 +7021,10 @@
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="24">
+      <c r="A7" s="25">
         <v>5</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="27" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
@@ -7067,7 +7133,7 @@
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>431</v>
@@ -7403,19 +7469,19 @@
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>46</v>
       </c>
     </row>
@@ -7793,7 +7859,7 @@
         <v>75</v>
       </c>
       <c r="D38" s="14"/>
-      <c r="E38" s="27" t="s">
+      <c r="E38" s="28" t="s">
         <v>125</v>
       </c>
     </row>
@@ -7893,7 +7959,7 @@
       <c r="D47" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="E47" s="22"/>
+      <c r="E47" s="23"/>
     </row>
     <row r="48" customFormat="1" spans="2:5">
       <c r="B48" s="4" t="s">
@@ -8133,7 +8199,7 @@
   <sheetPr/>
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -8215,7 +8281,7 @@
       <c r="C6" t="s">
         <v>197</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" ht="120" spans="2:6">
       <c r="B7" s="5" t="s">
@@ -8459,7 +8525,7 @@
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="22" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -8563,7 +8629,7 @@
         <v>253</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="22"/>
+      <c r="E9" s="23"/>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="5" t="s">
@@ -8691,7 +8757,7 @@
       <c r="C22" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="E22" s="20"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" ht="66" customHeight="1" spans="2:5">
       <c r="B23" t="s">
@@ -8755,7 +8821,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -8848,7 +8914,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" ht="63" customHeight="1" spans="2:4">
+    <row r="8" ht="63" customHeight="1" spans="2:6">
       <c r="B8" t="s">
         <v>299</v>
       </c>
@@ -8858,30 +8924,33 @@
       <c r="D8" s="10" t="s">
         <v>301</v>
       </c>
+      <c r="F8" s="19" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" ht="30" spans="2:5">
       <c r="B10" s="4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" ht="30" spans="2:5">
       <c r="B11" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>133</v>
@@ -8891,48 +8960,51 @@
     </row>
     <row r="12" ht="30" spans="2:5">
       <c r="B12" s="4" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" customFormat="1" ht="66" customHeight="1" spans="2:4">
+    <row r="13" customFormat="1" ht="66" customHeight="1" spans="2:6">
       <c r="B13" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>311</v>
+        <v>312</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="14" customFormat="1" spans="2:5">
       <c r="B14" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D14" s="10"/>
-      <c r="E14" s="20"/>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" customFormat="1" ht="30" spans="2:5">
       <c r="B15" s="4" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D15" s="10"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="21"/>
     </row>
     <row r="16" customFormat="1" ht="30" spans="2:5">
       <c r="B16" s="4" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>133</v>
@@ -8942,46 +9014,46 @@
     </row>
     <row r="17" customFormat="1" ht="30" spans="2:4">
       <c r="B17" s="4" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D17" s="10"/>
     </row>
     <row r="18" ht="60" spans="2:5">
       <c r="B18" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="19" ht="93" customHeight="1" spans="2:6">
       <c r="B19" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="2:6">
       <c r="B20" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="10"/>
       <c r="F20" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="21" customFormat="1" ht="50" customHeight="1" spans="2:6">
@@ -8990,7 +9062,7 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="10" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>98</v>
@@ -9002,7 +9074,7 @@
         <v>99</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D22" s="10"/>
       <c r="F22" s="4"/>
@@ -9012,7 +9084,7 @@
         <v>101</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="13" t="s">
@@ -9025,10 +9097,10 @@
         <v>84</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -9038,7 +9110,7 @@
         <v>80</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="4"/>
@@ -9049,7 +9121,7 @@
         <v>86</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="4"/>
@@ -9060,7 +9132,7 @@
         <v>88</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="4"/>
@@ -9071,7 +9143,7 @@
         <v>90</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="4"/>
@@ -9082,7 +9154,7 @@
         <v>92</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="4"/>
@@ -9093,7 +9165,7 @@
         <v>94</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="4"/>
@@ -9107,7 +9179,7 @@
         <v>189</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="32" customFormat="1" ht="46" customHeight="1" spans="2:4">
@@ -9115,7 +9187,7 @@
         <v>191</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="D32" s="14"/>
     </row>
@@ -9173,8 +9245,8 @@
       </c>
     </row>
     <row r="2" ht="45" spans="1:1">
-      <c r="A2" s="19" t="s">
-        <v>341</v>
+      <c r="A2" s="20" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -9183,7 +9255,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -9195,7 +9267,7 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -9215,7 +9287,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -9229,7 +9301,7 @@
         <v>53</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" ht="150" spans="2:5">
@@ -9237,38 +9309,38 @@
         <v>198</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="D8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" ht="70" customHeight="1" spans="2:4">
       <c r="B9" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="10" ht="30" spans="2:4">
       <c r="B10" s="5" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D10" s="10"/>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>216</v>
@@ -9278,43 +9350,43 @@
     </row>
     <row r="12" ht="30" spans="2:4">
       <c r="B12" s="5" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D12" s="10"/>
     </row>
     <row r="13" ht="38" customHeight="1" spans="2:4">
       <c r="B13" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="14" ht="30" spans="2:4">
       <c r="B14" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D14" s="10"/>
     </row>
     <row r="15" ht="153" customHeight="1" spans="2:5">
       <c r="B15" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="8" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" ht="75" spans="2:4">
@@ -9338,27 +9410,27 @@
     </row>
     <row r="18" ht="90" spans="2:5">
       <c r="B18" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="D18" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D19" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="20" spans="2:4">
@@ -9369,7 +9441,7 @@
         <v>189</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="21" ht="45" customHeight="1" spans="2:4">
@@ -9377,7 +9449,7 @@
         <v>191</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D21" s="14"/>
     </row>
@@ -9397,8 +9469,8 @@
   <sheetPr/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -9436,7 +9508,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -9449,23 +9521,21 @@
         <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="4" ht="46.5" spans="1:5">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="4" ht="78" spans="1:5">
       <c r="A4" s="1"/>
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>374</v>
-      </c>
-      <c r="D4" t="s">
         <v>375</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="19" t="s">
         <v>376</v>
       </c>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" customFormat="1" spans="1:6">
       <c r="A5" s="1"/>
@@ -9498,7 +9568,7 @@
         <v>53</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" ht="150" spans="2:5">
@@ -9509,10 +9579,10 @@
         <v>378</v>
       </c>
       <c r="D8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" ht="139" customHeight="1" spans="2:5">
@@ -9567,13 +9637,13 @@
     </row>
     <row r="14" ht="84" customHeight="1" spans="2:5">
       <c r="B14" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>388</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>389</v>
@@ -9581,7 +9651,7 @@
     </row>
     <row r="15" spans="2:5">
       <c r="B15" s="5" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>255</v>
@@ -9591,7 +9661,7 @@
     </row>
     <row r="16" spans="2:5">
       <c r="B16" s="5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>216</v>
@@ -9601,7 +9671,7 @@
     </row>
     <row r="17" ht="30" spans="2:5">
       <c r="B17" s="5" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>390</v>
@@ -9613,7 +9683,7 @@
     </row>
     <row r="18" ht="105" spans="2:5">
       <c r="B18" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>392</v>
@@ -9627,7 +9697,7 @@
     </row>
     <row r="19" ht="30" spans="2:3">
       <c r="B19" s="4" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>395</v>
@@ -9635,7 +9705,7 @@
     </row>
     <row r="20" ht="30" spans="2:3">
       <c r="B20" s="4" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C20" t="s">
         <v>216</v>
@@ -9706,11 +9776,11 @@
     </row>
     <row r="27" ht="210" spans="2:5">
       <c r="B27" s="5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E27" s="16" t="s">
         <v>407</v>
@@ -9729,14 +9799,14 @@
     </row>
     <row r="29" spans="2:6">
       <c r="B29" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D29" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="30" spans="2:4">
@@ -9755,7 +9825,7 @@
         <v>191</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D31" s="14"/>
     </row>
@@ -9829,7 +9899,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -9878,7 +9948,7 @@
         <v>413</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="8" ht="150" spans="2:5">
@@ -9889,10 +9959,10 @@
         <v>378</v>
       </c>
       <c r="D8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" ht="409" customHeight="1" spans="2:5">
@@ -9908,7 +9978,7 @@
     </row>
     <row r="10" ht="165" spans="2:5">
       <c r="B10" s="5" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>250</v>
@@ -9922,7 +9992,7 @@
     </row>
     <row r="11" ht="180" spans="2:5">
       <c r="B11" s="5" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C11" s="4"/>
       <c r="E11" s="11" t="s">
@@ -9931,7 +10001,7 @@
     </row>
     <row r="12" ht="150" spans="2:5">
       <c r="B12" s="5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C12" s="4"/>
       <c r="E12" s="11" t="s">
@@ -9970,11 +10040,11 @@
     </row>
     <row r="16" ht="210" spans="2:5">
       <c r="B16" s="5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E16" s="16" t="s">
         <v>407</v>
@@ -9993,16 +10063,16 @@
     </row>
     <row r="18" spans="2:6">
       <c r="B18" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="D18" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>420</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" ht="165" spans="2:5">
@@ -10032,7 +10102,7 @@
         <v>191</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D21" s="14"/>
     </row>

</xml_diff>